<commit_message>
Adding comparison of expression in 3 gene subsets: all genes, highest CAI, lowest CAI.
</commit_message>
<xml_diff>
--- a/Analysis/Outputs/Commonly_Enriched_GO_Terms.xlsx
+++ b/Analysis/Outputs/Commonly_Enriched_GO_Terms.xlsx
@@ -26,57 +26,57 @@
     <t xml:space="preserve">term_name</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0030204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:BP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chondroitin sulfate metabolic process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0030206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chondroitin sulfate biosynthetic process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0050650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chondroitin sulfate proteoglycan biosynthetic process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:1903510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mucopolysaccharide metabolic process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0050654</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chondroitin sulfate proteoglycan metabolic process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0080134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulation of response to stress</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:1902882</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:BP</t>
-  </si>
-  <si>
     <t xml:space="preserve">regulation of response to oxidative stress</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0080134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regulation of response to stress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0050654</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chondroitin sulfate proteoglycan metabolic process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0050650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chondroitin sulfate proteoglycan biosynthetic process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0030206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chondroitin sulfate biosynthetic process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0030204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chondroitin sulfate metabolic process</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:1902884</t>
   </si>
   <si>
     <t xml:space="preserve">positive regulation of response to oxidative stress</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:1903510</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mucopolysaccharide metabolic process</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0006023</t>
   </si>
   <si>
@@ -95,18 +95,18 @@
     <t xml:space="preserve">glycosaminoglycan metabolic process</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0030166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proteoglycan biosynthetic process</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0006029</t>
   </si>
   <si>
     <t xml:space="preserve">proteoglycan metabolic process</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0030166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proteoglycan biosynthetic process</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0006022</t>
   </si>
   <si>
@@ -131,18 +131,18 @@
     <t xml:space="preserve">sensory perception</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0006979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response to oxidative stress</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0009101</t>
   </si>
   <si>
     <t xml:space="preserve">glycoprotein biosynthetic process</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0006979</t>
-  </si>
-  <si>
-    <t xml:space="preserve">response to oxidative stress</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0009100</t>
   </si>
   <si>
@@ -233,18 +233,18 @@
     <t xml:space="preserve">transferase activity, transferring sulfur-containing groups</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0043043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peptide biosynthetic process</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0006412</t>
   </si>
   <si>
     <t xml:space="preserve">translation</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0043043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">peptide biosynthetic process</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0043604</t>
   </si>
   <si>
@@ -293,16 +293,16 @@
     <t xml:space="preserve">cellular macromolecule biosynthetic process</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0044249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cellular biosynthetic process</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0009059</t>
   </si>
   <si>
     <t xml:space="preserve">macromolecule biosynthetic process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0044249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cellular biosynthetic process</t>
   </si>
   <si>
     <t xml:space="preserve">GO:1901576</t>

</xml_diff>